<commit_message>
one hidden test case fixed
</commit_message>
<xml_diff>
--- a/lab1-linker/errors.xlsx
+++ b/lab1-linker/errors.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yucong/Study/opearting_system/linker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yucong/Study/opearting_system/lab1-linker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A611D800-8571-B246-88C5-062768DDDE1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071FCC5F-A743-A34E-8387-6F54217210CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1540" windowWidth="28240" windowHeight="17440" xr2:uid="{9270EC95-7B91-4C4F-AB8D-4564942E6234}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{9270EC95-7B91-4C4F-AB8D-4564942E6234}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>syntax error</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -187,44 +188,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">3 5 6 7 8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线 (正文)"/>
-        <charset val="134"/>
-      </rPr>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="4"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="4"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NUM_EXPECTED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -274,6 +237,22 @@
   </si>
   <si>
     <t>TOO_MANY_INSTR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">11 13 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checklist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 5 6 7 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -281,7 +260,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,19 +293,19 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线 (正文)"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -343,7 +322,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -353,11 +332,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,7 +658,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -685,7 +667,7 @@
     <col min="2" max="2" width="50.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="39.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="89.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" style="3" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -699,7 +681,7 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -707,7 +689,7 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -716,7 +698,7 @@
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -724,7 +706,7 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -733,7 +715,7 @@
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>4</v>
       </c>
     </row>
@@ -741,7 +723,7 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -750,7 +732,7 @@
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -758,7 +740,7 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -767,15 +749,15 @@
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>35</v>
+      <c r="E5" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -784,7 +766,7 @@
       <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>10</v>
       </c>
     </row>
@@ -792,7 +774,7 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -801,7 +783,7 @@
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -809,21 +791,24 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="4">
-        <v>20</v>
+      <c r="E8" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -832,7 +817,7 @@
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -840,7 +825,7 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -849,7 +834,7 @@
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>7</v>
       </c>
     </row>
@@ -860,10 +845,13 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>19</v>
       </c>
     </row>
@@ -874,10 +862,13 @@
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>19</v>
       </c>
     </row>
@@ -886,10 +877,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -897,10 +888,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
+      <c r="E15" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -908,10 +902,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
+      <c r="E16" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -919,10 +916,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -930,10 +927,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -941,10 +938,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -952,10 +949,144 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>49</v>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDA80AE-CFA1-8F42-837D-B13082FFDD1C}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>